<commit_message>
Finished code for assignment part 2
</commit_message>
<xml_diff>
--- a/Documentation/Assignment2.xlsx
+++ b/Documentation/Assignment2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\School\Year 2\Compiler Theory\CPS2000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD336791-22B1-4E29-91D8-4AE05AD40A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467FA2B2-82DB-410A-A228-D0F50B49501F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{CD838E60-5761-47BA-9DF5-194D02436BF0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{CD838E60-5761-47BA-9DF5-194D02436BF0}"/>
   </bookViews>
   <sheets>
     <sheet name="TX" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="79">
   <si>
     <t>START</t>
   </si>
@@ -254,6 +254,24 @@
   </si>
   <si>
     <t>S29</t>
+  </si>
+  <si>
+    <t>APOSTROPHE</t>
+  </si>
+  <si>
+    <t>S30</t>
+  </si>
+  <si>
+    <t>S31</t>
+  </si>
+  <si>
+    <t>S32</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>'</t>
   </si>
 </sst>
 </file>
@@ -303,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,6 +337,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,18 +661,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D27B639-3AD5-445C-AFBD-27629891CF59}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="22" max="22" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>6</v>
@@ -706,20 +735,23 @@
       <c r="U1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -784,19 +816,22 @@
         <v>72</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -872,8 +907,11 @@
       <c r="Y3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -949,8 +987,11 @@
       <c r="Y4" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1026,8 +1067,11 @@
       <c r="Y5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z5" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1103,8 +1147,11 @@
       <c r="Y6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z6" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1180,8 +1227,11 @@
       <c r="Y7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z7" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1257,8 +1307,11 @@
       <c r="Y8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z8" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1334,8 +1387,11 @@
       <c r="Y9" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z9" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1411,8 +1467,11 @@
       <c r="Y10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z10" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -1488,8 +1547,11 @@
       <c r="Y11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z11" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1565,8 +1627,11 @@
       <c r="Y12" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z12" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1642,8 +1707,11 @@
       <c r="Y13" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z13" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -1719,8 +1787,11 @@
       <c r="Y14" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z14" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1796,8 +1867,11 @@
       <c r="Y15" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z15" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1873,8 +1947,11 @@
       <c r="Y16" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z16" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1950,8 +2027,11 @@
       <c r="Y17" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z17" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
@@ -2027,8 +2107,11 @@
       <c r="Y18" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z18" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -2104,8 +2187,11 @@
       <c r="Y19" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z19" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>48</v>
       </c>
@@ -2181,8 +2267,11 @@
       <c r="Y20" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z20" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
@@ -2258,8 +2347,11 @@
       <c r="Y21" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z21" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
@@ -2335,8 +2427,11 @@
       <c r="Y22" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z22" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -2412,8 +2507,11 @@
       <c r="Y23" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z23" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
@@ -2489,8 +2587,11 @@
       <c r="Y24" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z24" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>57</v>
       </c>
@@ -2555,19 +2656,22 @@
         <v>16</v>
       </c>
       <c r="V25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="X25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X25" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="Y25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z25" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2632,19 +2736,22 @@
         <v>16</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="W26" s="2" t="s">
         <v>58</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="Y26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z26" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
@@ -2709,19 +2816,22 @@
         <v>16</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z27" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>60</v>
       </c>
@@ -2786,19 +2896,22 @@
         <v>16</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="W28" s="2" t="s">
         <v>58</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="Y28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z28" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -2874,8 +2987,11 @@
       <c r="Y29" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z29" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>71</v>
       </c>
@@ -2951,8 +3067,11 @@
       <c r="Y30" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z30" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>72</v>
       </c>
@@ -3028,33 +3147,249 @@
       <c r="Y31" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Z31" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2"/>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3065,15 +3400,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A8E78B-CC47-4727-81F1-3A21CF9C0653}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3164,8 +3499,17 @@
       <c r="AD1" t="s">
         <v>72</v>
       </c>
+      <c r="AE1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3255,6 +3599,15 @@
       </c>
       <c r="AD2" t="s">
         <v>70</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3265,15 +3618,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D8EC97-AC10-45DB-8C47-4D762AD7D5D6}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="21" max="21" width="12" style="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3334,20 +3690,23 @@
       <c r="T1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -3408,16 +3767,19 @@
       <c r="T2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>